<commit_message>
Remove app + cost alterations
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Items/artefacts.xlsx
+++ b/CoreRulebook/Data/Items/artefacts.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HPRPG\CoreRulebook\Data\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFC4D5D-4E40-4D41-971A-713AEE79F141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76F0A90-5667-43B2-9D64-FE9B49AF4E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1470" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -193,6 +201,36 @@
   </si>
   <si>
     <t xml:space="preserve">A sphere of perfect crystal – the manufacture of these objects is a carefully curated secret. A properly trained mind can use a crystal ball to peer through the mystic veil and learn about the universe. </t>
+  </si>
+  <si>
+    <t>GPBCost</t>
+  </si>
+  <si>
+    <t>BaseKnuts</t>
+  </si>
+  <si>
+    <t>Galleons</t>
+  </si>
+  <si>
+    <t>Sickles</t>
+  </si>
+  <si>
+    <t>Knuts</t>
+  </si>
+  <si>
+    <t>RoundSickles</t>
+  </si>
+  <si>
+    <t>RoundKnuts</t>
+  </si>
+  <si>
+    <t>StringGalleon</t>
+  </si>
+  <si>
+    <t>StringSickle</t>
+  </si>
+  <si>
+    <t>StringKnut</t>
   </si>
 </sst>
 </file>
@@ -549,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -561,7 +599,7 @@
     <col min="4" max="4" width="105.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,341 +612,1961 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>250</v>
+      <c r="C2" t="str">
+        <f>CONCATENATE(M2,N2,O2)</f>
+        <v>\galleon{5}~</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>250</v>
+      </c>
+      <c r="F2">
+        <f>E2*493/50</f>
+        <v>2465</v>
+      </c>
+      <c r="G2">
+        <f>FLOOR(F2/493,1)</f>
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <f>FLOOR((F2-493*G2)/29,1)</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>FLOOR((F2-493*G2-29*H2),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>IF(G2&gt;0,ROUND(H2/5,0)*5,H2)</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>IF(J2&gt;0,ROUND(I2/5,0)*5,I2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(G2&gt;0,CONCATENATE("\galleon{",G2,"}~"),"")</f>
+        <v>\galleon{5}~</v>
+      </c>
+      <c r="N2" t="str">
+        <f>IF(J2&gt;0,CONCATENATE("\sickle{",J2,"}~"),"")</f>
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <f>IF(G2&gt;0,"",IF(K2&gt;0,CONCATENATE("\knut{",K2,"}"),""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>2000</v>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C40" si="0">CONCATENATE(M3,N3,O3)</f>
+        <v>\galleon{40}~</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>2000</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F40" si="1">E3*493/50</f>
+        <v>19720</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G40" si="2">FLOOR(F3/493,1)</f>
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H40" si="3">FLOOR((F3-493*G3)/29,1)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I40" si="4">FLOOR((F3-493*G3-29*H3),1)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J40" si="5">IF(G3&gt;0,ROUND(H3/5,0)*5,H3)</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K40" si="6">IF(J3&gt;0,ROUND(I3/5,0)*5,I3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M40" si="7">IF(G3&gt;0,CONCATENATE("\galleon{",G3,"}~"),"")</f>
+        <v>\galleon{40}~</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N40" si="8">IF(J3&gt;0,CONCATENATE("\sickle{",J3,"}~"),"")</f>
+        <v/>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O40" si="9">IF(G3&gt;0,"",IF(K3&gt;0,CONCATENATE("\knut{",K3,"}"),""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>25000</v>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{500}~</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>25000</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>246500</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{500}~</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
-        <v>150</v>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{1}~</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>493</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{1}~</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
-        <v>50</v>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>\sickle{4}~</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>118.32</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="8"/>
+        <v>\sickle{4}~</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
-        <v>3000</v>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{60}~</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>3000</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>29580</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{60}~</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>5000</v>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{100}~</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>5000</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>49300</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{100}~</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
-        <v>15</v>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>\sickle{5}~</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>147.9</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="8"/>
+        <v>\sickle{5}~</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
-        <v>500</v>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{10}~</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>500</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>4930</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{10}~</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11">
-        <v>15</v>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>\sickle{1}~</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>29.58</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="8"/>
+        <v>\sickle{1}~</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12">
-        <v>12000</v>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{240}~</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>12000</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>118320</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{240}~</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
-        <v>250</v>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{1}~</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>493</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{1}~</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14">
-        <v>7500</v>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{150}~</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>7500</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>73950</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{150}~</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
-        <v>40</v>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>\sickle{15}~</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>44.2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>435.81200000000007</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="8"/>
+        <v>\sickle{15}~</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16">
-        <v>20000</v>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{400}~</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>20000</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>197200</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{400}~</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C17">
-        <v>800</v>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{16}~</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>800</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>7888</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{16}~</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C18">
-        <v>75</v>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{1}~\sickle{10}~</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>75</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>739.5</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{1}~</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="8"/>
+        <v>\sickle{10}~</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="C19">
-        <v>50</v>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{1}~</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>50</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>493</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{1}~</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>43</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C20">
-        <v>12000</v>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{24}~</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>1200</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>11832</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{24}~</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21">
-        <v>250</v>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{1}~</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>493</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{1}~</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>47</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="C22">
-        <v>12</v>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>\sickle{4}~</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>118.32</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="8"/>
+        <v>\sickle{4}~</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23">
-        <v>750</v>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{15}~</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>750</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>7395</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{15}~</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24">
-        <v>5000000</v>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{100000}~</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>5000000</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>49300000</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>100000</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{100000}~</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>53</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="C25">
-        <v>300</v>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>\galleon{6}~</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>54</v>
+      </c>
+      <c r="E25">
+        <v>300</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>2958</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="7"/>
+        <v>\galleon{6}~</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C26" t="str">
+        <f>CONCATENATE(M26,N26,O26)</f>
+        <v/>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="9"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>